<commit_message>
Removed Body variable and redefine some aggregates.
</commit_message>
<xml_diff>
--- a/input/book.xlsx
+++ b/input/book.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="linux">Отчет!$D$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Отчет!$1:$2</definedName>
     <definedName name="Заголовок">Отчет!$A$1:$E$2</definedName>
     <definedName name="Командировки">Отчет!$C$5</definedName>
     <definedName name="ОУ">Отчет!$A$5</definedName>
     <definedName name="Повтор">Отчет!$5:$6</definedName>
     <definedName name="Подвал">Отчет!$A$7:$E$8</definedName>
-    <definedName name="Тело">Отчет!$A$5:$E$6</definedName>
-    <definedName name="число_Людей">Отчет!$B$5</definedName>
+    <definedName name="число1">Отчет!$B$5</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -448,7 +448,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,15 +553,15 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7">
-        <f>SUM(B3,B5)</f>
+        <f>SUM(число1)</f>
+        <v>0.1</v>
+      </c>
+      <c r="C7">
+        <f>SUM(Командировки)</f>
         <v>0.2</v>
       </c>
-      <c r="C7">
-        <f t="shared" ref="C7:E7" si="0">SUM(C3,C5)</f>
-        <v>0.4</v>
-      </c>
       <c r="D7">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C7:E7" si="0">SUM(D3,D5)</f>
         <v>0.6</v>
       </c>
       <c r="E7">
@@ -579,8 +579,8 @@
         <v>5</v>
       </c>
       <c r="D8">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f>SUM(linux)</f>
+        <v>4</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>

</xml_diff>